<commit_message>
Adding test case for ticket OCEPROJECT-4905 (#217)
</commit_message>
<xml_diff>
--- a/test-data/sitewidesearch.xlsx
+++ b/test-data/sitewidesearch.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nci_workspace\qa_auto\wcms-qa-testing-framework\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DEDFD9E-FBDC-4035-B8D1-D5395DBA8424}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{074732FB-EEB8-47C5-BA38-5C9F114064AD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13515" xr2:uid="{C9E37E1E-A9C0-432B-8223-D4FB85813D47}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8210" tabRatio="706" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SitewideSearch" sheetId="1" r:id="rId1"/>
+    <sheet name="BestBet" sheetId="6" r:id="rId2"/>
+    <sheet name="BestBet_Definition" sheetId="7" r:id="rId3"/>
+    <sheet name="Definition" sheetId="3" r:id="rId4"/>
+    <sheet name="ContentTypeSearch" sheetId="2" r:id="rId5"/>
+    <sheet name="NoiseWords" sheetId="5" r:id="rId6"/>
+    <sheet name="SitewideSearch_ES" sheetId="4" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>mammography</t>
   </si>
@@ -39,16 +45,133 @@
     <t>Pancreas</t>
   </si>
   <si>
-    <t>small cell lung cancer</t>
-  </si>
-  <si>
-    <t>Cancer</t>
-  </si>
-  <si>
     <t>Keyword2</t>
   </si>
   <si>
     <t>Keyword1</t>
+  </si>
+  <si>
+    <t>Keyword</t>
+  </si>
+  <si>
+    <t>ContentType</t>
+  </si>
+  <si>
+    <t>Video Journey Into Nanotechnology</t>
+  </si>
+  <si>
+    <t>NCI At A Glance Infographic</t>
+  </si>
+  <si>
+    <t>Cancer and the Human Tumor Atlas Network</t>
+  </si>
+  <si>
+    <t>Understanding Cancer Prognosis Video Series</t>
+  </si>
+  <si>
+    <t>(Video Playlist)</t>
+  </si>
+  <si>
+    <t>(Video)</t>
+  </si>
+  <si>
+    <t>(Infographic)</t>
+  </si>
+  <si>
+    <t>BestBetKeywords</t>
+  </si>
+  <si>
+    <t>abdominal x-ray</t>
+  </si>
+  <si>
+    <t>breast cancer</t>
+  </si>
+  <si>
+    <t>biometrics</t>
+  </si>
+  <si>
+    <t>Cáncer colorrectal</t>
+  </si>
+  <si>
+    <t>Cáncer de próstata</t>
+  </si>
+  <si>
+    <t>Cáncer de vejiga</t>
+  </si>
+  <si>
+    <t>Versión para pacientes</t>
+  </si>
+  <si>
+    <t>Atezolizumab</t>
+  </si>
+  <si>
+    <t>La FDA aprueba el nivolumab</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
+    <t>of</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>bovine</t>
+  </si>
+  <si>
+    <t>Cardiopulmonary Syndromes</t>
+  </si>
+  <si>
+    <t>DefinitionKeywords</t>
+  </si>
+  <si>
+    <t>ipilimumab</t>
+  </si>
+  <si>
+    <t>NoiseWords</t>
+  </si>
+  <si>
+    <t>LiveHelp</t>
+  </si>
+  <si>
+    <t>BestBet_DefinitionKeywords</t>
+  </si>
+  <si>
+    <t>tumor</t>
+  </si>
+  <si>
+    <t>The Cancer Genome Atlas</t>
+  </si>
+  <si>
+    <t>glioblastoma</t>
+  </si>
+  <si>
+    <t>brain cancer</t>
   </si>
 </sst>
 </file>
@@ -66,7 +189,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,12 +204,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -94,15 +217,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,49 +556,352 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85333491-A4F8-4CEC-89F5-B1BA26A0B3FE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:A12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>0</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>